<commit_message>
Add upload data to table
</commit_message>
<xml_diff>
--- a/conf/Budget Categories.xlsx
+++ b/conf/Budget Categories.xlsx
@@ -5,13 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" name="category1" vbProcedure="false">Sheet4!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" name="category2" vbProcedure="false">Sheet4!$A$2:$B$6</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -214,6 +219,48 @@
   </si>
   <si>
     <t xml:space="preserve">Creadit Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select your choice:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pluto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jupiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
   </si>
 </sst>
 </file>
@@ -625,8 +672,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:J48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -637,7 +684,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="72.43"/>
@@ -1658,8 +1705,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="J2:J48 A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1775,8 +1822,8 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="1" sqref="J2:J48 C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2233,4 +2280,103 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1" type="list">
+      <formula1>category1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2" type="list">
+      <formula1>INDEX(category2,,MATCH(E1, category1,0))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>